<commit_message>
fix excel to json conversion
</commit_message>
<xml_diff>
--- a/timetables/Abe New Timetable09-09-2024.xlsx
+++ b/timetables/Abe New Timetable09-09-2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\colin\personal\ABE-Timetables\timetables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\colin\personal\ABE-Timetables\timetables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D4E3EE-E9BE-4BC4-A842-81B1B23E1175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6B7D7B-8D4B-4428-8B22-4AB488BF11D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E0491DF9-71E6-4376-A229-81EE0955FDFC}"/>
   </bookViews>
@@ -704,13 +704,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -765,13 +765,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>603250</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>8890</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -825,13 +825,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>590551</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>38102</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>36830</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>47910</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -861,8 +861,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4248151" y="2788922"/>
-          <a:ext cx="1275079" cy="192688"/>
+          <a:off x="3638551" y="2606042"/>
+          <a:ext cx="1275079" cy="207928"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1171,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAA28C8-4F9F-4B26-A06B-D1B28B012FB1}">
-  <dimension ref="B3:L65"/>
+  <dimension ref="B3:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,7 +1300,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1311,424 +1311,437 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="2" t="s">
+    <row r="15" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="L15" s="7" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1.05</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="I16" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="L16" s="13">
+        <v>1.25</v>
+      </c>
+    </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="8">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9">
+      <c r="B17" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1.4</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="I17" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="J17" s="12">
         <v>0.5</v>
       </c>
-      <c r="D17" s="9">
+      <c r="K17" s="12">
         <v>1.05</v>
       </c>
-      <c r="E17" s="9">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="I17" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="J17" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0.4</v>
-      </c>
       <c r="L17" s="13">
-        <v>1.25</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="14">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="C18" s="15">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="D18" s="15">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="15">
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="F18" s="16"/>
       <c r="I18" s="11">
-        <v>0.45</v>
+        <v>2</v>
       </c>
       <c r="J18" s="12">
-        <v>0.5</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="K18" s="12">
-        <v>1.05</v>
+        <v>2.35</v>
       </c>
       <c r="L18" s="13">
-        <v>1.55</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="14">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C19" s="15">
-        <v>1.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D19" s="15">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E19" s="15">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="F19" s="16"/>
       <c r="I19" s="11">
-        <v>2</v>
+        <v>2.35</v>
       </c>
       <c r="J19" s="12">
-        <v>2.0499999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="K19" s="12">
-        <v>2.35</v>
+        <v>3.05</v>
       </c>
       <c r="L19" s="13">
-        <v>3.15</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="14">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="15">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="D20" s="15">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
       <c r="E20" s="15">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="F20" s="16"/>
       <c r="I20" s="11">
-        <v>2.35</v>
+        <v>3</v>
       </c>
       <c r="J20" s="12">
-        <v>2.4</v>
+        <v>3.05</v>
       </c>
       <c r="K20" s="12">
-        <v>3.05</v>
+        <v>3.35</v>
       </c>
       <c r="L20" s="13">
-        <v>3.5</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="14">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C21" s="15">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="D21" s="15">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="E21" s="15">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="F21" s="16"/>
       <c r="I21" s="11">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="J21" s="12">
-        <v>3.05</v>
+        <v>3.45</v>
       </c>
       <c r="K21" s="12">
-        <v>3.35</v>
+        <v>4.05</v>
       </c>
       <c r="L21" s="13">
-        <v>4.1500000000000004</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="14">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
       <c r="C22" s="15">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="D22" s="15">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="E22" s="15">
-        <v>3.4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F22" s="16"/>
       <c r="I22" s="11">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="J22" s="12">
-        <v>3.45</v>
+        <v>4.05</v>
       </c>
       <c r="K22" s="12">
-        <v>4.05</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="L22" s="13">
-        <v>4.5</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C23" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="D23" s="15">
-        <v>4</v>
-      </c>
-      <c r="E23" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F23" s="16"/>
+        <v>5.45</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="17"/>
       <c r="I23" s="11">
-        <v>4</v>
+        <v>4.3</v>
       </c>
       <c r="J23" s="12">
-        <v>4.05</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="K23" s="12">
-        <v>4.3499999999999996</v>
+        <v>5.05</v>
       </c>
       <c r="L23" s="13">
-        <v>5.05</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="14">
         <v>5</v>
       </c>
-      <c r="C24" s="15">
-        <v>5.45</v>
-      </c>
+      <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="17"/>
+      <c r="E24" s="15">
+        <v>6.1</v>
+      </c>
+      <c r="F24" s="17">
+        <v>6.25</v>
+      </c>
       <c r="I24" s="11">
-        <v>4.3</v>
+        <v>5</v>
       </c>
       <c r="J24" s="12">
-        <v>4.3499999999999996</v>
+        <v>5.05</v>
       </c>
       <c r="K24" s="12">
-        <v>5.05</v>
+        <v>5.35</v>
       </c>
       <c r="L24" s="13">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="14">
-        <v>5</v>
-      </c>
-      <c r="C25" s="15"/>
+        <v>5.4</v>
+      </c>
+      <c r="C25" s="15">
+        <v>6.3</v>
+      </c>
       <c r="D25" s="15"/>
-      <c r="E25" s="15">
-        <v>6.1</v>
-      </c>
-      <c r="F25" s="17">
-        <v>6.25</v>
-      </c>
-      <c r="I25" s="11">
-        <v>5</v>
-      </c>
-      <c r="J25" s="12">
-        <v>5.05</v>
-      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="17"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
       <c r="K25" s="12">
-        <v>5.35</v>
+        <v>6.05</v>
       </c>
       <c r="L25" s="13">
-        <v>6.1</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="14">
-        <v>5.4</v>
-      </c>
-      <c r="C26" s="15">
-        <v>6.3</v>
-      </c>
+        <v>5.55</v>
+      </c>
+      <c r="C26" s="15"/>
       <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="17"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="12"/>
+      <c r="E26" s="15">
+        <v>7.1</v>
+      </c>
+      <c r="F26" s="17">
+        <v>7.25</v>
+      </c>
+      <c r="I26" s="11">
+        <v>6.15</v>
+      </c>
+      <c r="J26" s="12">
+        <v>6.2</v>
+      </c>
       <c r="K26" s="12">
-        <v>6.05</v>
+        <v>6.35</v>
       </c>
       <c r="L26" s="13">
-        <v>6.5</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="14">
-        <v>5.55</v>
+        <v>6.25</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15">
-        <v>7.1</v>
+        <v>7.4</v>
       </c>
       <c r="F27" s="17">
-        <v>7.25</v>
-      </c>
-      <c r="I27" s="11">
-        <v>6.15</v>
-      </c>
-      <c r="J27" s="12">
-        <v>6.2</v>
-      </c>
+        <v>7.55</v>
+      </c>
+      <c r="I27" s="11"/>
+      <c r="J27" s="12"/>
       <c r="K27" s="12">
-        <v>6.35</v>
+        <v>7.05</v>
       </c>
       <c r="L27" s="13">
-        <v>7.2</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="14">
-        <v>6.25</v>
+        <v>6.55</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15">
+        <v>8.1</v>
+      </c>
+      <c r="F28" s="17">
+        <v>8.25</v>
+      </c>
+      <c r="I28" s="11">
+        <v>7.15</v>
+      </c>
+      <c r="J28" s="12">
+        <v>7.2</v>
+      </c>
+      <c r="K28" s="12">
         <v>7.4</v>
       </c>
-      <c r="F28" s="17">
-        <v>7.55</v>
-      </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12">
-        <v>7.05</v>
-      </c>
       <c r="L28" s="13">
-        <v>7.5</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="14">
-        <v>6.55</v>
+        <v>7.25</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15">
+        <v>8.4</v>
+      </c>
+      <c r="F29" s="17">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="I29" s="11">
+        <v>7.45</v>
+      </c>
+      <c r="J29" s="12">
+        <v>7.55</v>
+      </c>
+      <c r="K29" s="12">
         <v>8.1</v>
       </c>
-      <c r="F29" s="17">
-        <v>8.25</v>
-      </c>
-      <c r="I29" s="11">
-        <v>7.15</v>
-      </c>
-      <c r="J29" s="12">
-        <v>7.2</v>
-      </c>
-      <c r="K29" s="12">
-        <v>7.4</v>
-      </c>
       <c r="L29" s="13">
-        <v>8.25</v>
+        <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="14">
-        <v>7.25</v>
-      </c>
-      <c r="C30" s="15"/>
+        <v>7.55</v>
+      </c>
+      <c r="C30" s="15">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15">
+        <v>9.25</v>
+      </c>
+      <c r="F30" s="17">
+        <v>9.4</v>
+      </c>
+      <c r="I30" s="11">
+        <v>8.15</v>
+      </c>
+      <c r="J30" s="12">
+        <f>SUM(I30+0.05)</f>
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="K30" s="12">
         <v>8.4</v>
       </c>
-      <c r="F30" s="17">
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="I30" s="11">
-        <v>7.45</v>
-      </c>
-      <c r="J30" s="12">
-        <v>7.55</v>
-      </c>
-      <c r="K30" s="12">
-        <v>8.1</v>
-      </c>
       <c r="L30" s="13">
-        <v>8.5500000000000007</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="14">
-        <v>7.55</v>
+        <v>8.25</v>
       </c>
       <c r="C31" s="15">
+        <v>9.15</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="17"/>
+      <c r="I31" s="11">
         <v>8.4499999999999993</v>
       </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15">
-        <v>9.25</v>
-      </c>
-      <c r="F31" s="17">
-        <v>9.4</v>
-      </c>
-      <c r="I31" s="11">
-        <v>8.15</v>
-      </c>
       <c r="J31" s="12">
-        <f>SUM(I31+0.05)</f>
-        <v>8.2000000000000011</v>
+        <f>SUM(I31+0.1)</f>
+        <v>8.5499999999999989</v>
       </c>
       <c r="K31" s="12">
-        <v>8.4</v>
+        <v>9.1</v>
       </c>
       <c r="L31" s="13">
-        <v>9.25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
@@ -1739,878 +1752,854 @@
         <v>9.15</v>
       </c>
       <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="17"/>
-      <c r="I32" s="11">
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="J32" s="12">
-        <f>SUM(I32+0.1)</f>
-        <v>8.5499999999999989</v>
-      </c>
+      <c r="E32" s="15">
+        <v>10</v>
+      </c>
+      <c r="F32" s="17">
+        <v>10.1</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="12"/>
       <c r="K32" s="12">
-        <v>9.1</v>
+        <v>9.4</v>
       </c>
       <c r="L32" s="13">
-        <v>10</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="14">
-        <v>8.25</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="C33" s="15">
-        <v>9.15</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15">
-        <v>10</v>
+        <v>10.3</v>
       </c>
       <c r="F33" s="17">
+        <v>10.4</v>
+      </c>
+      <c r="I33" s="11">
+        <v>9.35</v>
+      </c>
+      <c r="J33" s="12">
+        <v>9.4</v>
+      </c>
+      <c r="K33" s="12">
         <v>10.1</v>
       </c>
-      <c r="I33" s="11"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12">
-        <v>9.4</v>
-      </c>
       <c r="L33" s="13">
-        <v>10.199999999999999</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="14">
-        <v>8.5500000000000007</v>
+        <v>9.25</v>
       </c>
       <c r="C34" s="15">
-        <v>9.4499999999999993</v>
+        <v>10.15</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15">
-        <v>10.3</v>
+        <v>11</v>
       </c>
       <c r="F34" s="17">
+        <v>11.1</v>
+      </c>
+      <c r="I34" s="11">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="J34" s="12">
+        <v>10.1</v>
+      </c>
+      <c r="K34" s="12">
         <v>10.4</v>
       </c>
-      <c r="I34" s="11">
-        <v>9.35</v>
-      </c>
-      <c r="J34" s="12">
-        <v>9.4</v>
-      </c>
-      <c r="K34" s="12">
-        <v>10.1</v>
-      </c>
       <c r="L34" s="13">
-        <v>11</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="14">
-        <v>9.25</v>
+        <v>10</v>
       </c>
       <c r="C35" s="15">
-        <v>10.15</v>
+        <v>10.5</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15">
-        <v>11</v>
+        <v>11.3</v>
       </c>
       <c r="F35" s="17">
+        <v>11.4</v>
+      </c>
+      <c r="I35" s="11">
+        <f t="shared" ref="I35" si="0">SUM(I34+0.3)</f>
+        <v>10.350000000000001</v>
+      </c>
+      <c r="J35" s="12">
+        <v>10.4</v>
+      </c>
+      <c r="K35" s="12">
         <v>11.1</v>
       </c>
-      <c r="I35" s="11">
-        <v>10.050000000000001</v>
-      </c>
-      <c r="J35" s="12">
-        <v>10.1</v>
-      </c>
-      <c r="K35" s="12">
-        <v>10.4</v>
-      </c>
       <c r="L35" s="13">
-        <v>11.3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="14">
-        <v>10</v>
+        <v>10.3</v>
       </c>
       <c r="C36" s="15">
-        <v>10.5</v>
+        <v>11.2</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15">
-        <v>11.3</v>
+        <v>12</v>
       </c>
       <c r="F36" s="17">
+        <v>12.1</v>
+      </c>
+      <c r="I36" s="11">
+        <v>11.05</v>
+      </c>
+      <c r="J36" s="12">
+        <v>11.1</v>
+      </c>
+      <c r="K36" s="12">
         <v>11.4</v>
       </c>
-      <c r="I36" s="11">
-        <f t="shared" ref="I36" si="0">SUM(I35+0.3)</f>
-        <v>10.350000000000001</v>
-      </c>
-      <c r="J36" s="12">
-        <v>10.4</v>
-      </c>
-      <c r="K36" s="12">
-        <v>11.1</v>
-      </c>
       <c r="L36" s="13">
-        <v>12</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="14">
-        <v>10.3</v>
+        <v>11</v>
       </c>
       <c r="C37" s="15">
-        <v>11.2</v>
+        <v>11.5</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15">
-        <v>12</v>
+        <v>12.3</v>
       </c>
       <c r="F37" s="17">
+        <v>12.4</v>
+      </c>
+      <c r="I37" s="11">
+        <v>11.35</v>
+      </c>
+      <c r="J37" s="12">
+        <v>11.4</v>
+      </c>
+      <c r="K37" s="12">
         <v>12.1</v>
       </c>
-      <c r="I37" s="11">
-        <v>11.05</v>
-      </c>
-      <c r="J37" s="12">
-        <v>11.1</v>
-      </c>
-      <c r="K37" s="12">
-        <v>11.4</v>
-      </c>
       <c r="L37" s="13">
-        <v>12.3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="14">
-        <v>11</v>
+        <v>11.3</v>
       </c>
       <c r="C38" s="15">
-        <v>11.5</v>
+        <v>12.2</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15">
-        <v>12.3</v>
+        <v>13</v>
       </c>
       <c r="F38" s="17">
+        <v>13.1</v>
+      </c>
+      <c r="I38" s="11">
+        <v>12.05</v>
+      </c>
+      <c r="J38" s="12">
+        <v>12.1</v>
+      </c>
+      <c r="K38" s="12">
         <v>12.4</v>
       </c>
-      <c r="I38" s="11">
-        <v>11.35</v>
-      </c>
-      <c r="J38" s="12">
-        <v>11.4</v>
-      </c>
-      <c r="K38" s="12">
-        <v>12.1</v>
-      </c>
       <c r="L38" s="13">
-        <v>13</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="14">
-        <v>11.3</v>
+        <v>12</v>
       </c>
       <c r="C39" s="15">
-        <v>12.2</v>
+        <v>12.5</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15">
-        <v>13</v>
+        <v>13.3</v>
       </c>
       <c r="F39" s="17">
+        <v>13.4</v>
+      </c>
+      <c r="I39" s="11">
+        <v>12.35</v>
+      </c>
+      <c r="J39" s="12">
+        <v>12.4</v>
+      </c>
+      <c r="K39" s="12">
         <v>13.1</v>
       </c>
-      <c r="I39" s="11">
-        <v>12.05</v>
-      </c>
-      <c r="J39" s="12">
-        <v>12.1</v>
-      </c>
-      <c r="K39" s="12">
-        <v>12.4</v>
-      </c>
       <c r="L39" s="13">
-        <v>13.3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="14">
-        <v>12</v>
+        <v>12.3</v>
       </c>
       <c r="C40" s="15">
-        <v>12.5</v>
+        <v>13.2</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="15">
-        <v>13.3</v>
+        <v>14</v>
       </c>
       <c r="F40" s="17">
+        <v>14.1</v>
+      </c>
+      <c r="I40" s="11">
+        <v>13.05</v>
+      </c>
+      <c r="J40" s="12">
+        <v>13.1</v>
+      </c>
+      <c r="K40" s="12">
         <v>13.4</v>
       </c>
-      <c r="I40" s="11">
-        <v>12.35</v>
-      </c>
-      <c r="J40" s="12">
-        <v>12.4</v>
-      </c>
-      <c r="K40" s="12">
-        <v>13.1</v>
-      </c>
       <c r="L40" s="13">
-        <v>14</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="14">
-        <v>12.3</v>
+        <v>13</v>
       </c>
       <c r="C41" s="15">
-        <v>13.2</v>
+        <v>13.5</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="15">
-        <v>14</v>
+        <v>14.25</v>
       </c>
       <c r="F41" s="17">
+        <v>14.35</v>
+      </c>
+      <c r="I41" s="11">
+        <v>13.35</v>
+      </c>
+      <c r="J41" s="12">
+        <v>13.4</v>
+      </c>
+      <c r="K41" s="12">
         <v>14.1</v>
       </c>
-      <c r="I41" s="11">
-        <v>13.05</v>
-      </c>
-      <c r="J41" s="12">
-        <v>13.1</v>
-      </c>
-      <c r="K41" s="12">
-        <v>13.4</v>
-      </c>
       <c r="L41" s="13">
-        <v>14.3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="14">
-        <v>13</v>
+        <v>13.3</v>
       </c>
       <c r="C42" s="15">
-        <v>13.5</v>
+        <v>14.2</v>
       </c>
       <c r="D42" s="15"/>
-      <c r="E42" s="15">
-        <v>14.25</v>
-      </c>
-      <c r="F42" s="17">
-        <v>14.35</v>
-      </c>
+      <c r="E42" s="15"/>
+      <c r="F42" s="17"/>
       <c r="I42" s="11">
-        <v>13.35</v>
+        <v>14.05</v>
       </c>
       <c r="J42" s="12">
-        <v>13.4</v>
+        <v>14.1</v>
       </c>
       <c r="K42" s="12">
-        <v>14.1</v>
+        <v>14.4</v>
       </c>
       <c r="L42" s="13">
-        <v>15</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="14">
         <v>13.3</v>
       </c>
-      <c r="C43" s="15">
-        <v>14.2</v>
-      </c>
+      <c r="C43" s="15"/>
       <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="17"/>
+      <c r="E43" s="15">
+        <v>15</v>
+      </c>
+      <c r="F43" s="17">
+        <v>15.1</v>
+      </c>
       <c r="I43" s="11">
-        <v>14.05</v>
+        <v>14.3</v>
       </c>
       <c r="J43" s="12">
-        <v>14.1</v>
+        <v>14.35</v>
       </c>
       <c r="K43" s="12">
-        <v>14.4</v>
+        <v>15.1</v>
       </c>
       <c r="L43" s="13">
-        <v>15.3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" s="14">
-        <v>13.3</v>
-      </c>
-      <c r="C44" s="15"/>
+        <v>14</v>
+      </c>
+      <c r="C44" s="15">
+        <v>14.5</v>
+      </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15">
-        <v>15</v>
+        <v>15.3</v>
       </c>
       <c r="F44" s="17">
+        <v>15.4</v>
+      </c>
+      <c r="I44" s="11">
+        <v>15.05</v>
+      </c>
+      <c r="J44" s="12">
         <v>15.1</v>
       </c>
-      <c r="I44" s="11">
-        <v>14.3</v>
-      </c>
-      <c r="J44" s="12">
-        <v>14.35</v>
-      </c>
       <c r="K44" s="12">
-        <v>15.1</v>
+        <v>15.4</v>
       </c>
       <c r="L44" s="13">
-        <v>16</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="14">
-        <v>14</v>
+        <v>14.3</v>
       </c>
       <c r="C45" s="15">
-        <v>14.5</v>
+        <v>15.2</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="15">
-        <v>15.3</v>
+        <v>16</v>
       </c>
       <c r="F45" s="17">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="I45" s="11">
+        <v>15.35</v>
+      </c>
+      <c r="J45" s="12">
         <v>15.4</v>
       </c>
-      <c r="I45" s="11">
-        <v>15.05</v>
-      </c>
-      <c r="J45" s="12">
-        <v>15.1</v>
-      </c>
       <c r="K45" s="12">
-        <v>15.4</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="L45" s="13">
-        <v>16.3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="14">
-        <v>14.3</v>
+        <v>15</v>
       </c>
       <c r="C46" s="15">
-        <v>15.2</v>
+        <v>15.5</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="15">
-        <v>16</v>
+        <v>16.3</v>
       </c>
       <c r="F46" s="17">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I46" s="11">
+        <v>16.05</v>
+      </c>
+      <c r="J46" s="12">
         <v>16.100000000000001</v>
       </c>
-      <c r="I46" s="11">
-        <v>15.35</v>
-      </c>
-      <c r="J46" s="12">
-        <v>15.4</v>
-      </c>
       <c r="K46" s="12">
-        <v>16.100000000000001</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="L46" s="13">
-        <v>17</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="14">
-        <v>15</v>
+        <v>15.3</v>
       </c>
       <c r="C47" s="15">
-        <v>15.5</v>
+        <v>16.2</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="15">
-        <v>16.3</v>
+        <v>17</v>
       </c>
       <c r="F47" s="17">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="I47" s="11">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="J47" s="12">
         <v>16.399999999999999</v>
       </c>
-      <c r="I47" s="11">
-        <v>16.05</v>
-      </c>
-      <c r="J47" s="12">
-        <v>16.100000000000001</v>
-      </c>
       <c r="K47" s="12">
-        <v>16.399999999999999</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="L47" s="13">
-        <v>17.3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="14">
-        <v>15.3</v>
-      </c>
-      <c r="C48" s="15">
-        <v>16.2</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="15">
-        <v>17</v>
+        <v>17.3</v>
       </c>
       <c r="F48" s="17">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="I48" s="11">
+        <v>17.05</v>
+      </c>
+      <c r="J48" s="12">
         <v>17.100000000000001</v>
       </c>
-      <c r="I48" s="11">
-        <v>16.350000000000001</v>
-      </c>
-      <c r="J48" s="12">
-        <v>16.399999999999999</v>
-      </c>
       <c r="K48" s="12">
-        <v>17.100000000000001</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="L48" s="13">
-        <v>18</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B49" s="14">
         <v>16</v>
       </c>
-      <c r="C49" s="15"/>
+      <c r="C49" s="15">
+        <v>16.5</v>
+      </c>
       <c r="D49" s="15"/>
-      <c r="E49" s="15">
-        <v>17.3</v>
-      </c>
-      <c r="F49" s="17">
+      <c r="E49" s="15"/>
+      <c r="F49" s="17"/>
+      <c r="I49" s="11">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="J49" s="12">
         <v>17.399999999999999</v>
       </c>
-      <c r="I49" s="11">
-        <v>17.05</v>
-      </c>
-      <c r="J49" s="12">
-        <v>17.100000000000001</v>
-      </c>
       <c r="K49" s="12">
-        <v>17.399999999999999</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="L49" s="13">
-        <v>18.3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="14">
-        <v>16</v>
+        <v>16.3</v>
       </c>
       <c r="C50" s="15">
-        <v>16.5</v>
+        <v>17.2</v>
       </c>
       <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="17"/>
+      <c r="E50" s="15">
+        <v>18</v>
+      </c>
+      <c r="F50" s="17">
+        <v>18.100000000000001</v>
+      </c>
       <c r="I50" s="11">
-        <v>17.350000000000001</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="J50" s="12">
-        <v>17.399999999999999</v>
+        <v>18.149999999999999</v>
       </c>
       <c r="K50" s="12">
-        <v>18.100000000000001</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="L50" s="13">
-        <v>19</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B51" s="14">
-        <v>16.3</v>
+      <c r="B51" s="18">
+        <v>17</v>
       </c>
       <c r="C51" s="15">
-        <v>17.2</v>
+        <v>17.5</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="15">
-        <v>18</v>
+        <v>18.3</v>
       </c>
       <c r="F51" s="17">
-        <v>18.100000000000001</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="I51" s="11">
-        <v>18.100000000000001</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="J51" s="12">
-        <v>18.149999999999999</v>
-      </c>
-      <c r="K51" s="12">
         <v>18.399999999999999</v>
       </c>
+      <c r="K51" s="12"/>
       <c r="L51" s="13">
-        <v>19.3</v>
+        <v>19.45</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B52" s="18">
-        <v>17</v>
+      <c r="B52" s="14">
+        <v>17.3</v>
       </c>
       <c r="C52" s="15">
-        <v>17.5</v>
+        <v>18.2</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="15">
-        <v>18.3</v>
+        <v>18.55</v>
       </c>
       <c r="F52" s="17">
-        <v>18.399999999999999</v>
+        <v>19.05</v>
       </c>
       <c r="I52" s="11">
-        <v>18.350000000000001</v>
+        <v>19</v>
       </c>
       <c r="J52" s="12">
-        <v>18.399999999999999</v>
+        <v>19.05</v>
       </c>
       <c r="K52" s="12"/>
       <c r="L52" s="13">
-        <v>19.45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" s="14">
-        <v>17.3</v>
+        <v>18</v>
       </c>
       <c r="C53" s="15">
-        <v>18.2</v>
+        <v>18.5</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="15">
-        <v>18.55</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="F53" s="17">
-        <v>19.05</v>
+        <f t="shared" ref="F53" si="1">SUM(E53+0.15)</f>
+        <v>19.25</v>
       </c>
       <c r="I53" s="11">
-        <v>19</v>
+        <v>19.149999999999999</v>
       </c>
       <c r="J53" s="12">
-        <v>19.05</v>
-      </c>
-      <c r="K53" s="12"/>
+        <v>19.2</v>
+      </c>
+      <c r="K53" s="12">
+        <v>19.399999999999999</v>
+      </c>
       <c r="L53" s="13">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" s="14">
-        <v>18</v>
+        <v>18.3</v>
       </c>
       <c r="C54" s="15">
-        <v>18.5</v>
+        <v>19.2</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15">
-        <v>19.100000000000001</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="F54" s="17">
-        <f t="shared" ref="F54" si="1">SUM(E54+0.15)</f>
-        <v>19.25</v>
+        <v>19.5</v>
       </c>
       <c r="I54" s="11">
-        <v>19.149999999999999</v>
+        <v>19.45</v>
       </c>
       <c r="J54" s="12">
-        <v>19.2</v>
+        <v>19.5</v>
       </c>
       <c r="K54" s="12">
-        <v>19.399999999999999</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="L54" s="13">
-        <v>21</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" s="14">
-        <v>18.3</v>
+        <v>19</v>
       </c>
       <c r="C55" s="15">
-        <v>19.2</v>
+        <v>19.5</v>
       </c>
       <c r="D55" s="15"/>
-      <c r="E55" s="15">
-        <v>19.399999999999999</v>
+      <c r="E55" s="19">
+        <v>20.100000000000001</v>
       </c>
       <c r="F55" s="17">
-        <v>19.5</v>
+        <v>20.2</v>
       </c>
       <c r="I55" s="11">
-        <v>19.45</v>
+        <v>20.149999999999999</v>
       </c>
       <c r="J55" s="12">
-        <v>19.5</v>
+        <v>20.2</v>
       </c>
       <c r="K55" s="12">
-        <v>20.100000000000001</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="L55" s="13">
-        <v>21.3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" s="14">
-        <v>19</v>
+        <v>19.3</v>
       </c>
       <c r="C56" s="15">
-        <v>19.5</v>
+        <v>20.2</v>
       </c>
       <c r="D56" s="15"/>
-      <c r="E56" s="19">
-        <v>20.100000000000001</v>
+      <c r="E56" s="15">
+        <v>20.399999999999999</v>
       </c>
       <c r="F56" s="17">
-        <v>20.2</v>
+        <v>20.5</v>
       </c>
       <c r="I56" s="11">
-        <v>20.149999999999999</v>
+        <v>20.45</v>
       </c>
       <c r="J56" s="12">
-        <v>20.2</v>
+        <v>20.5</v>
       </c>
       <c r="K56" s="12">
-        <v>20.399999999999999</v>
+        <v>21.1</v>
       </c>
       <c r="L56" s="13">
-        <v>22</v>
+        <v>22.3</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="14">
-        <v>19.3</v>
+        <v>20</v>
       </c>
       <c r="C57" s="15">
-        <v>20.2</v>
+        <v>20.5</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="15">
-        <v>20.399999999999999</v>
+        <v>21.1</v>
       </c>
       <c r="F57" s="17">
-        <v>20.5</v>
+        <v>21.2</v>
       </c>
       <c r="I57" s="11">
-        <v>20.45</v>
+        <v>21.15</v>
       </c>
       <c r="J57" s="12">
-        <v>20.5</v>
+        <v>21.2</v>
       </c>
       <c r="K57" s="12">
-        <v>21.1</v>
+        <v>21.4</v>
       </c>
       <c r="L57" s="13">
-        <v>22.3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" s="14">
-        <v>20</v>
+        <v>20.3</v>
       </c>
       <c r="C58" s="15">
-        <v>20.5</v>
+        <v>21.2</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="15">
-        <v>21.1</v>
+        <v>21.4</v>
       </c>
       <c r="F58" s="17">
-        <v>21.2</v>
+        <v>21.5</v>
       </c>
       <c r="I58" s="11">
-        <v>21.15</v>
+        <v>21.45</v>
       </c>
       <c r="J58" s="12">
-        <v>21.2</v>
+        <v>21.5</v>
       </c>
       <c r="K58" s="12">
-        <v>21.4</v>
+        <v>22.1</v>
       </c>
       <c r="L58" s="13">
-        <v>23</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" s="14">
-        <v>20.3</v>
+        <v>21</v>
       </c>
       <c r="C59" s="15">
-        <v>21.2</v>
+        <v>21.5</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="15">
-        <v>21.4</v>
+        <v>22.1</v>
       </c>
       <c r="F59" s="17">
-        <v>21.5</v>
+        <v>21.2</v>
       </c>
       <c r="I59" s="11">
-        <v>21.45</v>
+        <v>22.15</v>
       </c>
       <c r="J59" s="12">
-        <v>21.5</v>
+        <v>22.2</v>
       </c>
       <c r="K59" s="12">
-        <v>22.1</v>
+        <v>22.4</v>
       </c>
       <c r="L59" s="13">
-        <v>23.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" s="14">
-        <v>21</v>
+        <v>21.3</v>
       </c>
       <c r="C60" s="15">
-        <v>21.5</v>
+        <v>22.2</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15">
-        <v>22.1</v>
+        <v>22.4</v>
       </c>
       <c r="F60" s="17">
-        <v>21.2</v>
+        <v>22.5</v>
       </c>
       <c r="I60" s="11">
-        <v>22.15</v>
+        <v>22.45</v>
       </c>
       <c r="J60" s="12">
-        <v>22.2</v>
+        <v>22.5</v>
       </c>
       <c r="K60" s="12">
-        <v>22.4</v>
+        <v>23.1</v>
       </c>
       <c r="L60" s="13">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B61" s="14">
-        <v>21.3</v>
+        <v>22</v>
       </c>
       <c r="C61" s="15">
-        <v>22.2</v>
+        <v>22.5</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61" s="15">
-        <v>22.4</v>
+        <v>23.1</v>
       </c>
       <c r="F61" s="17">
-        <v>22.5</v>
+        <v>23.2</v>
       </c>
       <c r="I61" s="11">
-        <v>22.45</v>
+        <v>23.15</v>
       </c>
       <c r="J61" s="12">
-        <v>22.5</v>
+        <v>23.2</v>
       </c>
       <c r="K61" s="12">
-        <v>23.1</v>
+        <v>23.4</v>
       </c>
       <c r="L61" s="13">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B62" s="14">
-        <v>22</v>
+        <v>22.3</v>
       </c>
       <c r="C62" s="15">
-        <v>22.5</v>
+        <v>23.2</v>
       </c>
       <c r="D62" s="15"/>
       <c r="E62" s="15">
-        <v>23.1</v>
+        <v>23.4</v>
       </c>
       <c r="F62" s="17">
-        <v>23.2</v>
-      </c>
-      <c r="I62" s="11">
-        <v>23.15</v>
-      </c>
-      <c r="J62" s="12">
-        <v>23.2</v>
-      </c>
-      <c r="K62" s="12">
-        <v>23.4</v>
-      </c>
-      <c r="L62" s="13">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>23.5</v>
+      </c>
+      <c r="I62" s="20">
+        <v>23.45</v>
+      </c>
+      <c r="J62" s="21">
+        <v>23.5</v>
+      </c>
+      <c r="K62" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="L62" s="22">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" s="14">
-        <v>22.3</v>
+        <v>23</v>
       </c>
       <c r="C63" s="15">
-        <v>23.2</v>
+        <v>23.5</v>
       </c>
       <c r="D63" s="15"/>
       <c r="E63" s="15">
-        <v>23.4</v>
+        <v>0.1</v>
       </c>
       <c r="F63" s="17">
-        <v>23.5</v>
-      </c>
-      <c r="I63" s="20">
-        <v>23.45</v>
-      </c>
-      <c r="J63" s="21">
-        <v>23.5</v>
-      </c>
-      <c r="K63" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="L63" s="22">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B64" s="14">
-        <v>23</v>
-      </c>
-      <c r="C64" s="15">
-        <v>23.5</v>
-      </c>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="F64" s="17">
         <v>0.2</v>
+      </c>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+    </row>
+    <row r="64" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="23">
+        <v>23.3</v>
+      </c>
+      <c r="C64" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24">
+        <v>0.4</v>
+      </c>
+      <c r="F64" s="25">
+        <v>0.5</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-    </row>
-    <row r="65" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="23">
-        <v>23.3</v>
-      </c>
-      <c r="C65" s="24">
-        <v>0.2</v>
-      </c>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24">
-        <v>0.4</v>
-      </c>
-      <c r="F65" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>